<commit_message>
Add all the importnat test cases
</commit_message>
<xml_diff>
--- a/cypress/fixtures/mainScreenData.xlsx
+++ b/cypress/fixtures/mainScreenData.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\p.somapala\OneDrive - ISM eGroup\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Exam\qa-exam-different\cypress\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2BD6C325-1B22-4C73-B842-3DADAF531AA5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CC1168F-0EB0-4141-AAF9-CBD882613D7D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-90" windowWidth="29040" windowHeight="15840" xr2:uid="{B973AC5D-3059-4D2B-BDA5-D6062AB5B96C}"/>
   </bookViews>
@@ -34,18 +34,27 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>TodoItemTitle</t>
   </si>
   <si>
-    <t>First</t>
-  </si>
-  <si>
-    <t>Second</t>
-  </si>
-  <si>
-    <t>Third</t>
+    <t>First todo</t>
+  </si>
+  <si>
+    <t>Second todo</t>
+  </si>
+  <si>
+    <t>Third todo</t>
+  </si>
+  <si>
+    <t>Fourth todo</t>
+  </si>
+  <si>
+    <t>Fifth todo</t>
+  </si>
+  <si>
+    <t>Sixth todo</t>
   </si>
 </sst>
 </file>
@@ -397,15 +406,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{722DAF58-2E4E-4773-B77B-DB81C2CD9162}">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:A7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="22" customWidth="1"/>
+    <col min="2" max="2" width="19.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
@@ -428,6 +438,21 @@
         <v>3</v>
       </c>
     </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>